<commit_message>
V2 w/ Marketing Mode & Docs
</commit_message>
<xml_diff>
--- a/EinteilungenTennisschuleKeller_2018Winter.xlsx
+++ b/EinteilungenTennisschuleKeller_2018Winter.xlsx
@@ -485,6 +485,9 @@
     <t>Mirella De Cia (4)</t>
   </si>
   <si>
+    <t>Nils Andres (17)</t>
+  </si>
+  <si>
     <t>Selina Hildenbrand (8)</t>
   </si>
   <si>
@@ -497,9 +500,6 @@
     <t>Noi Hliddal (14)</t>
   </si>
   <si>
-    <t>Nils Andres (17)</t>
-  </si>
-  <si>
     <t>Nico Schaffner (7)</t>
   </si>
   <si>
@@ -593,298 +593,298 @@
     <t>Richard Huser (16)</t>
   </si>
   <si>
+    <t>Leandro Lepore (21)</t>
+  </si>
+  <si>
+    <t>Raphaël Larisch (24)</t>
+  </si>
+  <si>
+    <t>Mark Csernyik (29)</t>
+  </si>
+  <si>
+    <t>Eva Stössel (8)</t>
+  </si>
+  <si>
+    <t>Emma Gasser (29)</t>
+  </si>
+  <si>
+    <t>Hanna Heinecke (47)</t>
+  </si>
+  <si>
+    <t>Fabio Gerstenberger (26)</t>
+  </si>
+  <si>
+    <t>Morris Künzler (42)</t>
+  </si>
+  <si>
     <t>Demian Farner (24)</t>
   </si>
   <si>
-    <t>Leandro Lepore (21)</t>
-  </si>
-  <si>
-    <t>Raphaël Larisch (24)</t>
-  </si>
-  <si>
-    <t>Mark Csernyik (29)</t>
-  </si>
-  <si>
-    <t>Eva Stössel (8)</t>
-  </si>
-  <si>
-    <t>Hanna Heinecke (47)</t>
-  </si>
-  <si>
-    <t>Fabio Gerstenberger (26)</t>
+    <t>Katharina Napravnik (18)</t>
+  </si>
+  <si>
+    <t>Dario Zwald (37)</t>
+  </si>
+  <si>
+    <t>Jan Waser (33)</t>
+  </si>
+  <si>
+    <t>Jan Lampert (27)</t>
+  </si>
+  <si>
+    <t>Cloe Bauer (26)</t>
+  </si>
+  <si>
+    <t>Aleksandar Filipovic (19)</t>
+  </si>
+  <si>
+    <t>Leonardo Castagna (16)</t>
+  </si>
+  <si>
+    <t>Riccardo Carli (41)</t>
+  </si>
+  <si>
+    <t>Arien Garcia (26)</t>
+  </si>
+  <si>
+    <t>Christian Buchenauer (7)</t>
+  </si>
+  <si>
+    <t>Ana Cadloni (7)</t>
+  </si>
+  <si>
+    <t>Chiara Maffei (7)</t>
+  </si>
+  <si>
+    <t>Michaela Andres (7)</t>
+  </si>
+  <si>
+    <t>Pamela Stankay (7)</t>
+  </si>
+  <si>
+    <t>Marin Angst (7)</t>
+  </si>
+  <si>
+    <t>Stefan Knup (1)</t>
+  </si>
+  <si>
+    <t>Gian Kemmler (4)</t>
+  </si>
+  <si>
+    <t>Lorenzo Lomartire (15)</t>
+  </si>
+  <si>
+    <t>Sophie Mini (7)</t>
+  </si>
+  <si>
+    <t>Marietta Knuth (4)</t>
+  </si>
+  <si>
+    <t>Halisa Saipi (2)</t>
+  </si>
+  <si>
+    <t>Nic Badertscher (6)</t>
+  </si>
+  <si>
+    <t>Eris Jakupi (21)</t>
+  </si>
+  <si>
+    <t>Fiona Schwarz (4)</t>
+  </si>
+  <si>
+    <t>Keira Schwarz (2)</t>
+  </si>
+  <si>
+    <t>Alysha Sivarajah (5)</t>
+  </si>
+  <si>
+    <t>Namuunaa Schmid (8)</t>
+  </si>
+  <si>
+    <t>Anna Napravnik (14)</t>
+  </si>
+  <si>
+    <t>Noelia Cadloni (8)</t>
+  </si>
+  <si>
+    <t>Mia Hagen (10)</t>
+  </si>
+  <si>
+    <t>Marco Schmidheiny (8)</t>
+  </si>
+  <si>
+    <t>Paul Teuber (5)</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Riaan Tomar (0)</t>
+  </si>
+  <si>
+    <t>Fabio De Vito (12)</t>
+  </si>
+  <si>
+    <t>Sinah Illi (7)</t>
+  </si>
+  <si>
+    <t>Yannik Egli (10)</t>
+  </si>
+  <si>
+    <t>Lionel Hagen (10)</t>
+  </si>
+  <si>
+    <t>Vittoria Müller (14)</t>
+  </si>
+  <si>
+    <t>Solana Zannini (2)</t>
+  </si>
+  <si>
+    <t>Dominic Dörig (11)</t>
+  </si>
+  <si>
+    <t>Denise Pfister (14)</t>
+  </si>
+  <si>
+    <t>Laura Marins (15)</t>
+  </si>
+  <si>
+    <t>Daniel Bolli (11)</t>
+  </si>
+  <si>
+    <t>Eric Knuth (8)</t>
+  </si>
+  <si>
+    <t>Ennio Sileno (12)</t>
+  </si>
+  <si>
+    <t>Simon Stirnemann (14)</t>
+  </si>
+  <si>
+    <t>Amalia Beradelli (14)</t>
+  </si>
+  <si>
+    <t>Fernando Ettlin (23)</t>
+  </si>
+  <si>
+    <t>Yves Meyer (22)</t>
+  </si>
+  <si>
+    <t>Mischa Giger (23)</t>
+  </si>
+  <si>
+    <t>Robin Sileno (22)</t>
+  </si>
+  <si>
+    <t>Nadine Riera (2)</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Marija Iveljic (7)</t>
+  </si>
+  <si>
+    <t>Minji Krempper (19)</t>
+  </si>
+  <si>
+    <t>Daniel Altherr (4)</t>
+  </si>
+  <si>
+    <t>Roger Trüb (4)</t>
+  </si>
+  <si>
+    <t>Claudia Gasser (6)</t>
+  </si>
+  <si>
+    <t>Berli Yuyu (1)</t>
+  </si>
+  <si>
+    <t>Roger Brand (0)</t>
+  </si>
+  <si>
+    <t>Mark Pfister (3)</t>
+  </si>
+  <si>
+    <t>Sophie Perret (10)</t>
+  </si>
+  <si>
+    <t>Lucas Cadloni (3)</t>
+  </si>
+  <si>
+    <t>Leandro Sperandio (11)</t>
+  </si>
+  <si>
+    <t>Jan Schaffner (3)</t>
+  </si>
+  <si>
+    <t>Ivan Alonso (3)</t>
+  </si>
+  <si>
+    <t>Julian Suppan (4)</t>
+  </si>
+  <si>
+    <t>Lorin Eggenberger (3)</t>
+  </si>
+  <si>
+    <t>Nicolas Bondolfi (5)</t>
+  </si>
+  <si>
+    <t>Noah Saillen (5)</t>
+  </si>
+  <si>
+    <t>Davi Rodrigues (5)</t>
+  </si>
+  <si>
+    <t>Liam Saillen (5)</t>
+  </si>
+  <si>
+    <t>David Pfister (9)</t>
+  </si>
+  <si>
+    <t>Robin Andres (28)</t>
+  </si>
+  <si>
+    <t>Yannick Krammer (33)</t>
+  </si>
+  <si>
+    <t>Katharina Meier (8)</t>
+  </si>
+  <si>
+    <t>Stefan Clas (8)</t>
+  </si>
+  <si>
+    <t>Brigitte Lamprecht (8)</t>
+  </si>
+  <si>
+    <t>Ana Neeracher (8)</t>
+  </si>
+  <si>
+    <t>Daniel Lakatos (13)</t>
+  </si>
+  <si>
+    <t>Loic Fäh (12)</t>
+  </si>
+  <si>
+    <t>Philip Meier (20)</t>
+  </si>
+  <si>
+    <t>Diego Gallo (20)</t>
+  </si>
+  <si>
+    <t>Sarina Messerli (20)</t>
+  </si>
+  <si>
+    <t>Cyrill Kloter (23)</t>
+  </si>
+  <si>
+    <t>Nadine Widmann (28)</t>
+  </si>
+  <si>
+    <t>Robin Sileno (25)</t>
   </si>
   <si>
     <t>Colin Meckes (33)</t>
-  </si>
-  <si>
-    <t>Morris Künzler (42)</t>
-  </si>
-  <si>
-    <t>Katharina Napravnik (18)</t>
-  </si>
-  <si>
-    <t>Dario Zwald (37)</t>
-  </si>
-  <si>
-    <t>Jan Waser (33)</t>
-  </si>
-  <si>
-    <t>Jan Lampert (27)</t>
-  </si>
-  <si>
-    <t>Cloe Bauer (26)</t>
-  </si>
-  <si>
-    <t>Aleksandar Filipovic (19)</t>
-  </si>
-  <si>
-    <t>Leonardo Castagna (16)</t>
-  </si>
-  <si>
-    <t>Riccardo Carli (41)</t>
-  </si>
-  <si>
-    <t>Arien Garcia (26)</t>
-  </si>
-  <si>
-    <t>Christian Buchenauer (7)</t>
-  </si>
-  <si>
-    <t>Ana Cadloni (7)</t>
-  </si>
-  <si>
-    <t>Chiara Maffei (7)</t>
-  </si>
-  <si>
-    <t>Michaela Andres (7)</t>
-  </si>
-  <si>
-    <t>Pamela Stankay (7)</t>
-  </si>
-  <si>
-    <t>Marin Angst (7)</t>
-  </si>
-  <si>
-    <t>Stefan Knup (1)</t>
-  </si>
-  <si>
-    <t>Gian Kemmler (4)</t>
-  </si>
-  <si>
-    <t>Lorenzo Lomartire (15)</t>
-  </si>
-  <si>
-    <t>Sophie Mini (7)</t>
-  </si>
-  <si>
-    <t>Marietta Knuth (4)</t>
-  </si>
-  <si>
-    <t>Halisa Saipi (2)</t>
-  </si>
-  <si>
-    <t>Nic Badertscher (6)</t>
-  </si>
-  <si>
-    <t>Eris Jakupi (21)</t>
-  </si>
-  <si>
-    <t>Fiona Schwarz (4)</t>
-  </si>
-  <si>
-    <t>Keira Schwarz (2)</t>
-  </si>
-  <si>
-    <t>Alysha Sivarajah (5)</t>
-  </si>
-  <si>
-    <t>Namuunaa Schmid (8)</t>
-  </si>
-  <si>
-    <t>Anna Napravnik (14)</t>
-  </si>
-  <si>
-    <t>Noelia Cadloni (8)</t>
-  </si>
-  <si>
-    <t>Marco Schmidheiny (8)</t>
-  </si>
-  <si>
-    <t>Yannik Egli (10)</t>
-  </si>
-  <si>
-    <t>Paul Teuber (5)</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>Riaan Tomar (0)</t>
-  </si>
-  <si>
-    <t>Fabio De Vito (12)</t>
-  </si>
-  <si>
-    <t>Sinah Illi (7)</t>
-  </si>
-  <si>
-    <t>Mia Hagen (10)</t>
-  </si>
-  <si>
-    <t>Lionel Hagen (10)</t>
-  </si>
-  <si>
-    <t>Vittoria Müller (14)</t>
-  </si>
-  <si>
-    <t>Solana Zannini (2)</t>
-  </si>
-  <si>
-    <t>Dominic Dörig (11)</t>
-  </si>
-  <si>
-    <t>Denise Pfister (14)</t>
-  </si>
-  <si>
-    <t>Laura Marins (15)</t>
-  </si>
-  <si>
-    <t>Daniel Bolli (11)</t>
-  </si>
-  <si>
-    <t>Eric Knuth (8)</t>
-  </si>
-  <si>
-    <t>Ennio Sileno (12)</t>
-  </si>
-  <si>
-    <t>Simon Stirnemann (14)</t>
-  </si>
-  <si>
-    <t>Amalia Beradelli (14)</t>
-  </si>
-  <si>
-    <t>Fernando Ettlin (23)</t>
-  </si>
-  <si>
-    <t>Yves Meyer (22)</t>
-  </si>
-  <si>
-    <t>Mischa Giger (23)</t>
-  </si>
-  <si>
-    <t>Robin Sileno (22)</t>
-  </si>
-  <si>
-    <t>Nadine Riera (2)</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>Marija Iveljic (7)</t>
-  </si>
-  <si>
-    <t>Minji Krempper (19)</t>
-  </si>
-  <si>
-    <t>Daniel Altherr (4)</t>
-  </si>
-  <si>
-    <t>Roger Trüb (4)</t>
-  </si>
-  <si>
-    <t>Claudia Gasser (6)</t>
-  </si>
-  <si>
-    <t>Berli Yuyu (1)</t>
-  </si>
-  <si>
-    <t>Roger Brand (0)</t>
-  </si>
-  <si>
-    <t>Mark Pfister (3)</t>
-  </si>
-  <si>
-    <t>Sophie Perret (10)</t>
-  </si>
-  <si>
-    <t>Lucas Cadloni (3)</t>
-  </si>
-  <si>
-    <t>Leandro Sperandio (11)</t>
-  </si>
-  <si>
-    <t>Jan Schaffner (3)</t>
-  </si>
-  <si>
-    <t>Ivan Alonso (3)</t>
-  </si>
-  <si>
-    <t>Julian Suppan (4)</t>
-  </si>
-  <si>
-    <t>Lorin Eggenberger (3)</t>
-  </si>
-  <si>
-    <t>Nicolas Bondolfi (5)</t>
-  </si>
-  <si>
-    <t>Noah Saillen (5)</t>
-  </si>
-  <si>
-    <t>Davi Rodrigues (5)</t>
-  </si>
-  <si>
-    <t>Liam Saillen (5)</t>
-  </si>
-  <si>
-    <t>David Pfister (9)</t>
-  </si>
-  <si>
-    <t>Robin Andres (28)</t>
-  </si>
-  <si>
-    <t>Yannick Krammer (33)</t>
-  </si>
-  <si>
-    <t>Katharina Meier (8)</t>
-  </si>
-  <si>
-    <t>Stefan Clas (8)</t>
-  </si>
-  <si>
-    <t>Brigitte Lamprecht (8)</t>
-  </si>
-  <si>
-    <t>Ana Neeracher (8)</t>
-  </si>
-  <si>
-    <t>Daniel Lakatos (13)</t>
-  </si>
-  <si>
-    <t>Loic Fäh (12)</t>
-  </si>
-  <si>
-    <t>Philip Meier (20)</t>
-  </si>
-  <si>
-    <t>Diego Gallo (20)</t>
-  </si>
-  <si>
-    <t>Sarina Messerli (20)</t>
-  </si>
-  <si>
-    <t>Cyrill Kloter (23)</t>
-  </si>
-  <si>
-    <t>Nadine Widmann (28)</t>
-  </si>
-  <si>
-    <t>Emma Gasser (29)</t>
-  </si>
-  <si>
-    <t>Robin Sileno (25)</t>
   </si>
   <si>
     <t>Mischa Giger (1)</t>
@@ -14172,7 +14172,7 @@
       <c r="AA86"/>
       <c r="AB86" s="1811"/>
       <c r="AC86" t="s" s="97">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD86" t="n">
         <v>4.0</v>
@@ -15051,7 +15051,7 @@
         <v>145</v>
       </c>
       <c r="D94" t="n" s="1957">
-        <v>2008.0</v>
+        <v>2009.0</v>
       </c>
       <c r="E94"/>
       <c r="F94"/>
@@ -15198,7 +15198,7 @@
         <v>145</v>
       </c>
       <c r="D95" t="n" s="1976">
-        <v>2006.0</v>
+        <v>2008.0</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
@@ -15277,7 +15277,7 @@
       <c r="AU95"/>
       <c r="AV95" s="1987"/>
       <c r="AW95" t="s" s="189">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AX95" t="n">
         <v>4.0</v>
@@ -15289,7 +15289,7 @@
         <v>2012.0</v>
       </c>
       <c r="BA95" t="s" s="193">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="BB95" t="n">
         <v>4.0</v>
@@ -15345,7 +15345,7 @@
         <v>145</v>
       </c>
       <c r="D96" t="n" s="1995">
-        <v>2012.0</v>
+        <v>2006.0</v>
       </c>
       <c r="E96"/>
       <c r="F96"/>
@@ -15492,7 +15492,7 @@
         <v>145</v>
       </c>
       <c r="D97" t="n" s="2014">
-        <v>2010.0</v>
+        <v>2012.0</v>
       </c>
       <c r="E97"/>
       <c r="F97"/>
@@ -15536,7 +15536,7 @@
         <v>188</v>
       </c>
       <c r="AF97" t="n" s="2021">
-        <v>2010.0</v>
+        <v>2011.0</v>
       </c>
       <c r="AG97"/>
       <c r="AH97"/>
@@ -15659,7 +15659,7 @@
         <v>188</v>
       </c>
       <c r="AF98" t="n" s="2040">
-        <v>2009.0</v>
+        <v>2010.0</v>
       </c>
       <c r="AG98"/>
       <c r="AH98"/>
@@ -16124,7 +16124,7 @@
         <v>145</v>
       </c>
       <c r="D103" t="n" s="2128">
-        <v>2009.0</v>
+        <v>2010.0</v>
       </c>
       <c r="E103" t="s" s="35">
         <v>165</v>
@@ -16434,10 +16434,10 @@
         <v>188</v>
       </c>
       <c r="AJ105" t="n" s="2174">
-        <v>2011.0</v>
+        <v>2009.0</v>
       </c>
       <c r="AK105" t="s" s="152">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL105" t="n">
         <v>4.0</v>
@@ -17134,13 +17134,13 @@
         <v>4.0</v>
       </c>
       <c r="O112" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="P112" t="n" s="2302">
-        <v>2007.0</v>
+        <v>2006.0</v>
       </c>
       <c r="Q112" t="s" s="65">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R112" t="n">
         <v>1.0</v>
@@ -17297,10 +17297,10 @@
         <v>4.0</v>
       </c>
       <c r="O113" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="P113" t="n" s="2321">
-        <v>2006.0</v>
+        <v>2004.0</v>
       </c>
       <c r="Q113"/>
       <c r="R113"/>
@@ -17444,10 +17444,10 @@
         <v>4.0</v>
       </c>
       <c r="O114" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="P114" t="n" s="2340">
-        <v>2004.0</v>
+        <v>2007.0</v>
       </c>
       <c r="Q114"/>
       <c r="R114"/>
@@ -17569,7 +17569,7 @@
       <c r="K115"/>
       <c r="L115" s="2358"/>
       <c r="M115" t="s" s="64">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="N115" t="n">
         <v>4.0</v>
@@ -17578,7 +17578,7 @@
         <v>167</v>
       </c>
       <c r="P115" t="n" s="2359">
-        <v>2007.0</v>
+        <v>2004.0</v>
       </c>
       <c r="Q115"/>
       <c r="R115"/>
@@ -18201,7 +18201,7 @@
         <v>1998.0</v>
       </c>
       <c r="M121" t="s" s="66">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N121" t="n">
         <v>4.0</v>
@@ -18213,16 +18213,16 @@
         <v>2001.0</v>
       </c>
       <c r="Q121" t="s" s="70">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R121" t="n">
         <v>4.0</v>
       </c>
       <c r="S121" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="T121" t="n" s="2474">
-        <v>2005.0</v>
+        <v>2007.0</v>
       </c>
       <c r="U121" t="s" s="74">
         <v>205</v>
@@ -18396,25 +18396,25 @@
       <c r="K122"/>
       <c r="L122" s="2491"/>
       <c r="M122" t="s" s="67">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N122" t="n">
         <v>4.0</v>
       </c>
       <c r="O122" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="P122" t="n" s="2492">
         <v>2001.0</v>
       </c>
       <c r="Q122" t="s" s="71">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R122" t="n">
         <v>4.0</v>
       </c>
       <c r="S122" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="T122" t="n" s="2493">
         <v>2005.0</v>
@@ -18575,7 +18575,7 @@
       <c r="K123"/>
       <c r="L123" s="2510"/>
       <c r="M123" t="s" s="68">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N123" t="n">
         <v>4.0</v>
@@ -18584,19 +18584,19 @@
         <v>143</v>
       </c>
       <c r="P123" t="n" s="2511">
-        <v>1998.0</v>
+        <v>2001.0</v>
       </c>
       <c r="Q123" t="s" s="72">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="R123" t="n">
         <v>4.0</v>
       </c>
       <c r="S123" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="T123" t="n" s="2512">
-        <v>2004.0</v>
+        <v>2005.0</v>
       </c>
       <c r="U123"/>
       <c r="V123"/>
@@ -18746,7 +18746,7 @@
       <c r="K124"/>
       <c r="L124" s="2529"/>
       <c r="M124" t="s" s="69">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N124" t="n">
         <v>4.0</v>
@@ -19613,10 +19613,10 @@
         <v>4.0</v>
       </c>
       <c r="AQ131" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="AR131" t="n" s="2670">
-        <v>2001.0</v>
+        <v>1999.0</v>
       </c>
       <c r="AS131" t="s">
         <v>2</v>
@@ -19763,7 +19763,7 @@
         <v>143</v>
       </c>
       <c r="AR132" t="n" s="2689">
-        <v>1999.0</v>
+        <v>1998.0</v>
       </c>
       <c r="AS132" t="s">
         <v>2</v>
@@ -19901,7 +19901,7 @@
         <v>2006.0</v>
       </c>
       <c r="AO133" t="s" s="173">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AP133" t="n">
         <v>4.0</v>

</xml_diff>

<commit_message>
PrioPlayers Attempt - failed
</commit_message>
<xml_diff>
--- a/EinteilungenTennisschuleKeller_2018Winter.xlsx
+++ b/EinteilungenTennisschuleKeller_2018Winter.xlsx
@@ -485,21 +485,21 @@
     <t>Mirella De Cia (4)</t>
   </si>
   <si>
+    <t>Selina Hildenbrand (8)</t>
+  </si>
+  <si>
+    <t>Erisa Jakupi (6)</t>
+  </si>
+  <si>
+    <t>Livio Hildenbrand (14)</t>
+  </si>
+  <si>
+    <t>Noi Hliddal (14)</t>
+  </si>
+  <si>
     <t>Nils Andres (17)</t>
   </si>
   <si>
-    <t>Selina Hildenbrand (8)</t>
-  </si>
-  <si>
-    <t>Erisa Jakupi (6)</t>
-  </si>
-  <si>
-    <t>Livio Hildenbrand (14)</t>
-  </si>
-  <si>
-    <t>Noi Hliddal (14)</t>
-  </si>
-  <si>
     <t>Nico Schaffner (7)</t>
   </si>
   <si>
@@ -593,298 +593,298 @@
     <t>Richard Huser (16)</t>
   </si>
   <si>
+    <t>Demian Farner (24)</t>
+  </si>
+  <si>
     <t>Leandro Lepore (21)</t>
   </si>
   <si>
     <t>Raphaël Larisch (24)</t>
   </si>
   <si>
+    <t>Eva Stössel (8)</t>
+  </si>
+  <si>
+    <t>Hanna Heinecke (47)</t>
+  </si>
+  <si>
+    <t>Fabio Gerstenberger (26)</t>
+  </si>
+  <si>
+    <t>Colin Meckes (33)</t>
+  </si>
+  <si>
+    <t>Morris Künzler (42)</t>
+  </si>
+  <si>
+    <t>Dario Zwald (37)</t>
+  </si>
+  <si>
     <t>Mark Csernyik (29)</t>
   </si>
   <si>
-    <t>Eva Stössel (8)</t>
+    <t>Jan Waser (33)</t>
+  </si>
+  <si>
+    <t>Yannick Krammer (33)</t>
+  </si>
+  <si>
+    <t>Jan Lampert (27)</t>
+  </si>
+  <si>
+    <t>Cloe Bauer (26)</t>
+  </si>
+  <si>
+    <t>Aleksandar Filipovic (19)</t>
+  </si>
+  <si>
+    <t>Leonardo Castagna (16)</t>
+  </si>
+  <si>
+    <t>Riccardo Carli (41)</t>
+  </si>
+  <si>
+    <t>Arien Garcia (26)</t>
+  </si>
+  <si>
+    <t>Christian Buchenauer (7)</t>
+  </si>
+  <si>
+    <t>Ana Cadloni (7)</t>
+  </si>
+  <si>
+    <t>Chiara Maffei (7)</t>
+  </si>
+  <si>
+    <t>Michaela Andres (7)</t>
+  </si>
+  <si>
+    <t>Pamela Stankay (7)</t>
+  </si>
+  <si>
+    <t>Marin Angst (7)</t>
+  </si>
+  <si>
+    <t>Stefan Knup (1)</t>
+  </si>
+  <si>
+    <t>Gian Kemmler (4)</t>
+  </si>
+  <si>
+    <t>Lorenzo Lomartire (15)</t>
+  </si>
+  <si>
+    <t>Sophie Mini (7)</t>
+  </si>
+  <si>
+    <t>Marietta Knuth (4)</t>
+  </si>
+  <si>
+    <t>Halisa Saipi (2)</t>
+  </si>
+  <si>
+    <t>Nic Badertscher (6)</t>
+  </si>
+  <si>
+    <t>Eris Jakupi (21)</t>
+  </si>
+  <si>
+    <t>Fiona Schwarz (4)</t>
+  </si>
+  <si>
+    <t>Keira Schwarz (2)</t>
+  </si>
+  <si>
+    <t>Alysha Sivarajah (5)</t>
+  </si>
+  <si>
+    <t>Namuunaa Schmid (8)</t>
+  </si>
+  <si>
+    <t>Anna Napravnik (14)</t>
+  </si>
+  <si>
+    <t>Noelia Cadloni (8)</t>
+  </si>
+  <si>
+    <t>Marco Schmidheiny (8)</t>
+  </si>
+  <si>
+    <t>Yannik Egli (10)</t>
+  </si>
+  <si>
+    <t>Paul Teuber (5)</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Riaan Tomar (0)</t>
+  </si>
+  <si>
+    <t>Fabio De Vito (12)</t>
+  </si>
+  <si>
+    <t>Sinah Illi (7)</t>
+  </si>
+  <si>
+    <t>Mia Hagen (10)</t>
+  </si>
+  <si>
+    <t>Lionel Hagen (10)</t>
+  </si>
+  <si>
+    <t>Vittoria Müller (14)</t>
+  </si>
+  <si>
+    <t>Solana Zannini (2)</t>
+  </si>
+  <si>
+    <t>Dominic Dörig (11)</t>
+  </si>
+  <si>
+    <t>Denise Pfister (14)</t>
+  </si>
+  <si>
+    <t>Laura Marins (15)</t>
+  </si>
+  <si>
+    <t>Daniel Bolli (11)</t>
+  </si>
+  <si>
+    <t>Eric Knuth (8)</t>
+  </si>
+  <si>
+    <t>Ennio Sileno (12)</t>
+  </si>
+  <si>
+    <t>Simon Stirnemann (14)</t>
+  </si>
+  <si>
+    <t>Amalia Beradelli (14)</t>
+  </si>
+  <si>
+    <t>Yves Meyer (22)</t>
+  </si>
+  <si>
+    <t>Mischa Giger (23)</t>
+  </si>
+  <si>
+    <t>Robin Sileno (22)</t>
+  </si>
+  <si>
+    <t>Nadine Riera (2)</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Marija Iveljic (7)</t>
+  </si>
+  <si>
+    <t>Minji Krempper (19)</t>
+  </si>
+  <si>
+    <t>Daniel Altherr (4)</t>
+  </si>
+  <si>
+    <t>Roger Trüb (4)</t>
+  </si>
+  <si>
+    <t>Claudia Gasser (6)</t>
+  </si>
+  <si>
+    <t>Berli Yuyu (1)</t>
+  </si>
+  <si>
+    <t>Roger Brand (0)</t>
+  </si>
+  <si>
+    <t>Mark Pfister (3)</t>
+  </si>
+  <si>
+    <t>Sophie Perret (10)</t>
+  </si>
+  <si>
+    <t>Lucas Cadloni (3)</t>
+  </si>
+  <si>
+    <t>Leandro Sperandio (11)</t>
+  </si>
+  <si>
+    <t>Jan Schaffner (3)</t>
+  </si>
+  <si>
+    <t>Ivan Alonso (3)</t>
+  </si>
+  <si>
+    <t>Julian Suppan (4)</t>
+  </si>
+  <si>
+    <t>Lorin Eggenberger (3)</t>
+  </si>
+  <si>
+    <t>Nicolas Bondolfi (5)</t>
+  </si>
+  <si>
+    <t>Noah Saillen (5)</t>
+  </si>
+  <si>
+    <t>Davi Rodrigues (5)</t>
+  </si>
+  <si>
+    <t>Liam Saillen (5)</t>
+  </si>
+  <si>
+    <t>Daniel Lakatos (13)</t>
+  </si>
+  <si>
+    <t>David Pfister (9)</t>
+  </si>
+  <si>
+    <t>Robin Andres (28)</t>
+  </si>
+  <si>
+    <t>Katharina Meier (8)</t>
+  </si>
+  <si>
+    <t>Stefan Clas (8)</t>
+  </si>
+  <si>
+    <t>Brigitte Lamprecht (8)</t>
+  </si>
+  <si>
+    <t>Ana Neeracher (8)</t>
+  </si>
+  <si>
+    <t>Katharina Napravnik (18)</t>
+  </si>
+  <si>
+    <t>Loic Fäh (12)</t>
+  </si>
+  <si>
+    <t>Philip Meier (20)</t>
+  </si>
+  <si>
+    <t>Diego Gallo (20)</t>
+  </si>
+  <si>
+    <t>Sarina Messerli (20)</t>
+  </si>
+  <si>
+    <t>Cyrill Kloter (23)</t>
+  </si>
+  <si>
+    <t>Fernando Ettlin (23)</t>
+  </si>
+  <si>
+    <t>Nadine Widmann (28)</t>
   </si>
   <si>
     <t>Emma Gasser (29)</t>
   </si>
   <si>
-    <t>Hanna Heinecke (47)</t>
-  </si>
-  <si>
-    <t>Fabio Gerstenberger (26)</t>
-  </si>
-  <si>
-    <t>Morris Künzler (42)</t>
-  </si>
-  <si>
-    <t>Demian Farner (24)</t>
-  </si>
-  <si>
-    <t>Katharina Napravnik (18)</t>
-  </si>
-  <si>
-    <t>Dario Zwald (37)</t>
-  </si>
-  <si>
-    <t>Jan Waser (33)</t>
-  </si>
-  <si>
-    <t>Jan Lampert (27)</t>
-  </si>
-  <si>
-    <t>Cloe Bauer (26)</t>
-  </si>
-  <si>
-    <t>Aleksandar Filipovic (19)</t>
-  </si>
-  <si>
-    <t>Leonardo Castagna (16)</t>
-  </si>
-  <si>
-    <t>Riccardo Carli (41)</t>
-  </si>
-  <si>
-    <t>Arien Garcia (26)</t>
-  </si>
-  <si>
-    <t>Christian Buchenauer (7)</t>
-  </si>
-  <si>
-    <t>Ana Cadloni (7)</t>
-  </si>
-  <si>
-    <t>Chiara Maffei (7)</t>
-  </si>
-  <si>
-    <t>Michaela Andres (7)</t>
-  </si>
-  <si>
-    <t>Pamela Stankay (7)</t>
-  </si>
-  <si>
-    <t>Marin Angst (7)</t>
-  </si>
-  <si>
-    <t>Stefan Knup (1)</t>
-  </si>
-  <si>
-    <t>Gian Kemmler (4)</t>
-  </si>
-  <si>
-    <t>Lorenzo Lomartire (15)</t>
-  </si>
-  <si>
-    <t>Sophie Mini (7)</t>
-  </si>
-  <si>
-    <t>Marietta Knuth (4)</t>
-  </si>
-  <si>
-    <t>Halisa Saipi (2)</t>
-  </si>
-  <si>
-    <t>Nic Badertscher (6)</t>
-  </si>
-  <si>
-    <t>Eris Jakupi (21)</t>
-  </si>
-  <si>
-    <t>Fiona Schwarz (4)</t>
-  </si>
-  <si>
-    <t>Keira Schwarz (2)</t>
-  </si>
-  <si>
-    <t>Alysha Sivarajah (5)</t>
-  </si>
-  <si>
-    <t>Namuunaa Schmid (8)</t>
-  </si>
-  <si>
-    <t>Anna Napravnik (14)</t>
-  </si>
-  <si>
-    <t>Noelia Cadloni (8)</t>
-  </si>
-  <si>
-    <t>Mia Hagen (10)</t>
-  </si>
-  <si>
-    <t>Marco Schmidheiny (8)</t>
-  </si>
-  <si>
-    <t>Paul Teuber (5)</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>Riaan Tomar (0)</t>
-  </si>
-  <si>
-    <t>Fabio De Vito (12)</t>
-  </si>
-  <si>
-    <t>Sinah Illi (7)</t>
-  </si>
-  <si>
-    <t>Yannik Egli (10)</t>
-  </si>
-  <si>
-    <t>Lionel Hagen (10)</t>
-  </si>
-  <si>
-    <t>Vittoria Müller (14)</t>
-  </si>
-  <si>
-    <t>Solana Zannini (2)</t>
-  </si>
-  <si>
-    <t>Dominic Dörig (11)</t>
-  </si>
-  <si>
-    <t>Denise Pfister (14)</t>
-  </si>
-  <si>
-    <t>Laura Marins (15)</t>
-  </si>
-  <si>
-    <t>Daniel Bolli (11)</t>
-  </si>
-  <si>
-    <t>Eric Knuth (8)</t>
-  </si>
-  <si>
-    <t>Ennio Sileno (12)</t>
-  </si>
-  <si>
-    <t>Simon Stirnemann (14)</t>
-  </si>
-  <si>
-    <t>Amalia Beradelli (14)</t>
-  </si>
-  <si>
-    <t>Fernando Ettlin (23)</t>
-  </si>
-  <si>
-    <t>Yves Meyer (22)</t>
-  </si>
-  <si>
-    <t>Mischa Giger (23)</t>
-  </si>
-  <si>
-    <t>Robin Sileno (22)</t>
-  </si>
-  <si>
-    <t>Nadine Riera (2)</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>Marija Iveljic (7)</t>
-  </si>
-  <si>
-    <t>Minji Krempper (19)</t>
-  </si>
-  <si>
-    <t>Daniel Altherr (4)</t>
-  </si>
-  <si>
-    <t>Roger Trüb (4)</t>
-  </si>
-  <si>
-    <t>Claudia Gasser (6)</t>
-  </si>
-  <si>
-    <t>Berli Yuyu (1)</t>
-  </si>
-  <si>
-    <t>Roger Brand (0)</t>
-  </si>
-  <si>
-    <t>Mark Pfister (3)</t>
-  </si>
-  <si>
-    <t>Sophie Perret (10)</t>
-  </si>
-  <si>
-    <t>Lucas Cadloni (3)</t>
-  </si>
-  <si>
-    <t>Leandro Sperandio (11)</t>
-  </si>
-  <si>
-    <t>Jan Schaffner (3)</t>
-  </si>
-  <si>
-    <t>Ivan Alonso (3)</t>
-  </si>
-  <si>
-    <t>Julian Suppan (4)</t>
-  </si>
-  <si>
-    <t>Lorin Eggenberger (3)</t>
-  </si>
-  <si>
-    <t>Nicolas Bondolfi (5)</t>
-  </si>
-  <si>
-    <t>Noah Saillen (5)</t>
-  </si>
-  <si>
-    <t>Davi Rodrigues (5)</t>
-  </si>
-  <si>
-    <t>Liam Saillen (5)</t>
-  </si>
-  <si>
-    <t>David Pfister (9)</t>
-  </si>
-  <si>
-    <t>Robin Andres (28)</t>
-  </si>
-  <si>
-    <t>Yannick Krammer (33)</t>
-  </si>
-  <si>
-    <t>Katharina Meier (8)</t>
-  </si>
-  <si>
-    <t>Stefan Clas (8)</t>
-  </si>
-  <si>
-    <t>Brigitte Lamprecht (8)</t>
-  </si>
-  <si>
-    <t>Ana Neeracher (8)</t>
-  </si>
-  <si>
-    <t>Daniel Lakatos (13)</t>
-  </si>
-  <si>
-    <t>Loic Fäh (12)</t>
-  </si>
-  <si>
-    <t>Philip Meier (20)</t>
-  </si>
-  <si>
-    <t>Diego Gallo (20)</t>
-  </si>
-  <si>
-    <t>Sarina Messerli (20)</t>
-  </si>
-  <si>
-    <t>Cyrill Kloter (23)</t>
-  </si>
-  <si>
-    <t>Nadine Widmann (28)</t>
-  </si>
-  <si>
     <t>Robin Sileno (25)</t>
-  </si>
-  <si>
-    <t>Colin Meckes (33)</t>
   </si>
   <si>
     <t>Mischa Giger (1)</t>
@@ -4517,7 +4517,7 @@
     <col min="14" max="14" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="3.34375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="5.49609375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="23.32421875" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="22.37109375" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="3.34375" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="5.49609375" customWidth="true" bestFit="true"/>
@@ -4537,7 +4537,7 @@
     <col min="34" max="34" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="3.34375" customWidth="true" bestFit="true"/>
     <col min="36" max="36" width="5.49609375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="22.87109375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="23.32421875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="3.34375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="5.49609375" customWidth="true" bestFit="true"/>
@@ -5745,7 +5745,7 @@
       <c r="AI13"/>
       <c r="AJ13" s="426"/>
       <c r="AK13" t="s" s="132">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AL13" t="n">
         <v>1.0</v>
@@ -6762,7 +6762,7 @@
       <c r="AI22"/>
       <c r="AJ22" s="597"/>
       <c r="AK22" t="s" s="133">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AL22" t="n">
         <v>1.0</v>
@@ -7803,7 +7803,7 @@
       <c r="AI31"/>
       <c r="AJ31" s="768"/>
       <c r="AK31" t="s" s="134">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AL31" t="n">
         <v>1.0</v>
@@ -9909,7 +9909,7 @@
       <c r="AI49"/>
       <c r="AJ49" s="1110"/>
       <c r="AK49" t="s" s="136">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AL49" t="n">
         <v>1.0</v>
@@ -10926,7 +10926,7 @@
       <c r="AI58"/>
       <c r="AJ58" s="1281"/>
       <c r="AK58" t="s" s="137">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AL58" t="n">
         <v>1.0</v>
@@ -12300,7 +12300,7 @@
       <c r="W70"/>
       <c r="X70" s="1506"/>
       <c r="Y70" t="s" s="90">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Z70" t="n">
         <v>4.0</v>
@@ -12996,7 +12996,7 @@
         <v>1998.0</v>
       </c>
       <c r="AK76" t="s" s="138">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AL76" t="n">
         <v>4.0</v>
@@ -13131,7 +13131,7 @@
       <c r="AI77"/>
       <c r="AJ77" s="1642"/>
       <c r="AK77" t="s" s="139">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AL77" t="n">
         <v>4.0</v>
@@ -13258,7 +13258,7 @@
       <c r="AI78"/>
       <c r="AJ78" s="1661"/>
       <c r="AK78" t="s" s="140">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AL78" t="n">
         <v>4.0</v>
@@ -13377,7 +13377,7 @@
       <c r="AI79"/>
       <c r="AJ79" s="1680"/>
       <c r="AK79" t="s" s="141">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AL79" t="n">
         <v>4.0</v>
@@ -14061,7 +14061,7 @@
       <c r="AI85"/>
       <c r="AJ85" s="1794"/>
       <c r="AK85" t="s" s="142">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AL85" t="n">
         <v>8.0</v>
@@ -14172,7 +14172,7 @@
       <c r="AA86"/>
       <c r="AB86" s="1811"/>
       <c r="AC86" t="s" s="97">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="AD86" t="n">
         <v>4.0</v>
@@ -14188,7 +14188,7 @@
       <c r="AI86"/>
       <c r="AJ86" s="1813"/>
       <c r="AK86" t="s" s="143">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AL86" t="n">
         <v>8.0</v>
@@ -14315,7 +14315,7 @@
       <c r="AI87"/>
       <c r="AJ87" s="1832"/>
       <c r="AK87" t="s" s="144">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AL87" t="n">
         <v>8.0</v>
@@ -14442,7 +14442,7 @@
       <c r="AI88"/>
       <c r="AJ88" s="1851"/>
       <c r="AK88" t="s" s="145">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL88" t="n">
         <v>8.0</v>
@@ -15051,7 +15051,7 @@
         <v>145</v>
       </c>
       <c r="D94" t="n" s="1957">
-        <v>2009.0</v>
+        <v>2008.0</v>
       </c>
       <c r="E94"/>
       <c r="F94"/>
@@ -15110,7 +15110,7 @@
       <c r="AI94"/>
       <c r="AJ94" s="1965"/>
       <c r="AK94" t="s" s="146">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL94" t="n">
         <v>4.0</v>
@@ -15198,7 +15198,7 @@
         <v>145</v>
       </c>
       <c r="D95" t="n" s="1976">
-        <v>2008.0</v>
+        <v>2006.0</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
@@ -15257,7 +15257,7 @@
       <c r="AI95"/>
       <c r="AJ95" s="1984"/>
       <c r="AK95" t="s" s="147">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AL95" t="n">
         <v>4.0</v>
@@ -15277,7 +15277,7 @@
       <c r="AU95"/>
       <c r="AV95" s="1987"/>
       <c r="AW95" t="s" s="189">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AX95" t="n">
         <v>4.0</v>
@@ -15289,7 +15289,7 @@
         <v>2012.0</v>
       </c>
       <c r="BA95" t="s" s="193">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="BB95" t="n">
         <v>4.0</v>
@@ -15345,7 +15345,7 @@
         <v>145</v>
       </c>
       <c r="D96" t="n" s="1995">
-        <v>2006.0</v>
+        <v>2012.0</v>
       </c>
       <c r="E96"/>
       <c r="F96"/>
@@ -15404,7 +15404,7 @@
       <c r="AI96"/>
       <c r="AJ96" s="2003"/>
       <c r="AK96" t="s" s="148">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AL96" t="n">
         <v>4.0</v>
@@ -15492,7 +15492,7 @@
         <v>145</v>
       </c>
       <c r="D97" t="n" s="2014">
-        <v>2012.0</v>
+        <v>2010.0</v>
       </c>
       <c r="E97"/>
       <c r="F97"/>
@@ -15536,14 +15536,14 @@
         <v>188</v>
       </c>
       <c r="AF97" t="n" s="2021">
-        <v>2011.0</v>
+        <v>2010.0</v>
       </c>
       <c r="AG97"/>
       <c r="AH97"/>
       <c r="AI97"/>
       <c r="AJ97" s="2022"/>
       <c r="AK97" t="s" s="149">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AL97" t="n">
         <v>4.0</v>
@@ -15659,7 +15659,7 @@
         <v>188</v>
       </c>
       <c r="AF98" t="n" s="2040">
-        <v>2010.0</v>
+        <v>2009.0</v>
       </c>
       <c r="AG98"/>
       <c r="AH98"/>
@@ -16124,7 +16124,7 @@
         <v>145</v>
       </c>
       <c r="D103" t="n" s="2128">
-        <v>2010.0</v>
+        <v>2009.0</v>
       </c>
       <c r="E103" t="s" s="35">
         <v>165</v>
@@ -16191,16 +16191,16 @@
         <v>2009.0</v>
       </c>
       <c r="AK103" t="s" s="150">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AL103" t="n">
         <v>4.0</v>
       </c>
       <c r="AM103" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="AN103" t="n" s="2137">
-        <v>2008.0</v>
+        <v>2009.0</v>
       </c>
       <c r="AO103"/>
       <c r="AP103"/>
@@ -16314,16 +16314,16 @@
         <v>2012.0</v>
       </c>
       <c r="AK104" t="s" s="151">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AL104" t="n">
         <v>4.0</v>
       </c>
       <c r="AM104" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="AN104" t="n" s="2156">
-        <v>2007.0</v>
+        <v>2008.0</v>
       </c>
       <c r="AO104"/>
       <c r="AP104"/>
@@ -16434,19 +16434,19 @@
         <v>188</v>
       </c>
       <c r="AJ105" t="n" s="2174">
-        <v>2009.0</v>
+        <v>2011.0</v>
       </c>
       <c r="AK105" t="s" s="152">
-        <v>193</v>
+        <v>276</v>
       </c>
       <c r="AL105" t="n">
         <v>4.0</v>
       </c>
       <c r="AM105" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="AN105" t="n" s="2175">
-        <v>2006.0</v>
+        <v>2007.0</v>
       </c>
       <c r="AO105"/>
       <c r="AP105"/>
@@ -16560,13 +16560,13 @@
         <v>2010.0</v>
       </c>
       <c r="AK106" t="s" s="153">
-        <v>277</v>
+        <v>194</v>
       </c>
       <c r="AL106" t="n">
         <v>4.0</v>
       </c>
       <c r="AM106" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="AN106" t="n" s="2194">
         <v>2006.0</v>
@@ -17134,10 +17134,10 @@
         <v>4.0</v>
       </c>
       <c r="O112" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="P112" t="n" s="2302">
-        <v>2006.0</v>
+        <v>2007.0</v>
       </c>
       <c r="Q112" t="s" s="65">
         <v>196</v>
@@ -17184,7 +17184,7 @@
       <c r="AI112"/>
       <c r="AJ112" s="2307"/>
       <c r="AK112" t="s" s="154">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AL112" t="n">
         <v>4.0</v>
@@ -17216,7 +17216,7 @@
         <v>2005.0</v>
       </c>
       <c r="BA112" t="s" s="200">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BB112" t="n">
         <v>4.0</v>
@@ -17297,10 +17297,10 @@
         <v>4.0</v>
       </c>
       <c r="O113" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="P113" t="n" s="2321">
-        <v>2004.0</v>
+        <v>2006.0</v>
       </c>
       <c r="Q113"/>
       <c r="R113"/>
@@ -17339,7 +17339,7 @@
       <c r="AI113"/>
       <c r="AJ113" s="2326"/>
       <c r="AK113" t="s" s="155">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AL113" t="n">
         <v>4.0</v>
@@ -17444,10 +17444,10 @@
         <v>4.0</v>
       </c>
       <c r="O114" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="P114" t="n" s="2340">
-        <v>2007.0</v>
+        <v>2004.0</v>
       </c>
       <c r="Q114"/>
       <c r="R114"/>
@@ -17478,7 +17478,7 @@
       <c r="AI114"/>
       <c r="AJ114" s="2345"/>
       <c r="AK114" t="s" s="156">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AL114" t="n">
         <v>4.0</v>
@@ -17609,7 +17609,7 @@
       <c r="AI115"/>
       <c r="AJ115" s="2364"/>
       <c r="AK115" t="s" s="157">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AL115" t="n">
         <v>4.0</v>
@@ -18222,7 +18222,7 @@
         <v>143</v>
       </c>
       <c r="T121" t="n" s="2474">
-        <v>2007.0</v>
+        <v>2005.0</v>
       </c>
       <c r="U121" t="s" s="74">
         <v>205</v>
@@ -18255,10 +18255,10 @@
         <v>4.0</v>
       </c>
       <c r="AE121" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="AF121" t="n" s="2477">
-        <v>1999.0</v>
+        <v>2001.0</v>
       </c>
       <c r="AG121" t="s" s="128">
         <v>205</v>
@@ -18273,7 +18273,7 @@
         <v>2008.0</v>
       </c>
       <c r="AK121" t="s" s="158">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AL121" t="n">
         <v>4.0</v>
@@ -18282,10 +18282,10 @@
         <v>148</v>
       </c>
       <c r="AN121" t="n" s="2479">
-        <v>2009.0</v>
+        <v>2005.0</v>
       </c>
       <c r="AO121" t="s" s="162">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AP121" t="n">
         <v>3.0</v>
@@ -18402,7 +18402,7 @@
         <v>4.0</v>
       </c>
       <c r="O122" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="P122" t="n" s="2492">
         <v>2001.0</v>
@@ -18414,10 +18414,10 @@
         <v>4.0</v>
       </c>
       <c r="S122" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="T122" t="n" s="2493">
-        <v>2005.0</v>
+        <v>2007.0</v>
       </c>
       <c r="U122" t="s" s="75">
         <v>206</v>
@@ -18450,17 +18450,17 @@
         <v>4.0</v>
       </c>
       <c r="AE122" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="AF122" t="n" s="2496">
-        <v>2001.0</v>
+        <v>1998.0</v>
       </c>
       <c r="AG122"/>
       <c r="AH122"/>
       <c r="AI122"/>
       <c r="AJ122" s="2497"/>
       <c r="AK122" t="s" s="159">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AL122" t="n">
         <v>4.0</v>
@@ -18472,7 +18472,7 @@
         <v>2008.0</v>
       </c>
       <c r="AO122" t="s" s="163">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AP122" t="n">
         <v>3.0</v>
@@ -18584,7 +18584,7 @@
         <v>143</v>
       </c>
       <c r="P123" t="n" s="2511">
-        <v>2001.0</v>
+        <v>1998.0</v>
       </c>
       <c r="Q123" t="s" s="72">
         <v>203</v>
@@ -18593,7 +18593,7 @@
         <v>4.0</v>
       </c>
       <c r="S123" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="T123" t="n" s="2512">
         <v>2005.0</v>
@@ -18624,7 +18624,7 @@
         <v>143</v>
       </c>
       <c r="AF123" t="n" s="2515">
-        <v>1998.0</v>
+        <v>1999.0</v>
       </c>
       <c r="AG123"/>
       <c r="AH123"/>
@@ -18643,7 +18643,7 @@
         <v>2006.0</v>
       </c>
       <c r="AO123" t="s" s="164">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AP123" t="n">
         <v>3.0</v>
@@ -18764,10 +18764,10 @@
         <v>4.0</v>
       </c>
       <c r="S124" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="T124" t="n" s="2531">
-        <v>2005.0</v>
+        <v>2006.0</v>
       </c>
       <c r="U124"/>
       <c r="V124"/>
@@ -18786,7 +18786,7 @@
         <v>1998.0</v>
       </c>
       <c r="AC124" t="s" s="127">
-        <v>253</v>
+        <v>200</v>
       </c>
       <c r="AD124" t="n">
         <v>4.0</v>
@@ -19410,19 +19410,19 @@
       <c r="W130"/>
       <c r="X130" s="2646"/>
       <c r="Y130" t="s" s="129">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z130" t="n">
         <v>4.0</v>
       </c>
       <c r="AA130" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AB130" t="n" s="2647">
         <v>1998.0</v>
       </c>
       <c r="AC130" t="s" s="130">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AD130" t="n">
         <v>4.0</v>
@@ -19440,7 +19440,7 @@
       <c r="AI130"/>
       <c r="AJ130" s="2649"/>
       <c r="AK130" t="s" s="166">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AL130" t="n">
         <v>4.0</v>
@@ -19452,16 +19452,16 @@
         <v>2003.0</v>
       </c>
       <c r="AO130" t="s" s="170">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AP130" t="n">
         <v>4.0</v>
       </c>
       <c r="AQ130" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="AR130" t="n" s="2651">
-        <v>2000.0</v>
+        <v>1999.0</v>
       </c>
       <c r="AS130" t="s">
         <v>2</v>
@@ -19577,7 +19577,7 @@
       <c r="AA131"/>
       <c r="AB131" s="2666"/>
       <c r="AC131" t="s" s="131">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AD131" t="n">
         <v>4.0</v>
@@ -19607,16 +19607,16 @@
         <v>2005.0</v>
       </c>
       <c r="AO131" t="s" s="171">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AP131" t="n">
         <v>4.0</v>
       </c>
       <c r="AQ131" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="AR131" t="n" s="2670">
-        <v>1999.0</v>
+        <v>2000.0</v>
       </c>
       <c r="AS131" t="s">
         <v>2</v>
@@ -19754,16 +19754,16 @@
         <v>2006.0</v>
       </c>
       <c r="AO132" t="s" s="172">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AP132" t="n">
         <v>4.0</v>
       </c>
       <c r="AQ132" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="AR132" t="n" s="2689">
-        <v>1998.0</v>
+        <v>2001.0</v>
       </c>
       <c r="AS132" t="s">
         <v>2</v>
@@ -19901,7 +19901,7 @@
         <v>2006.0</v>
       </c>
       <c r="AO133" t="s" s="173">
-        <v>200</v>
+        <v>290</v>
       </c>
       <c r="AP133" t="n">
         <v>4.0</v>

</xml_diff>